<commit_message>
Fixed and implemented outputting _all_ wage details for employees when '2' selected from the menu
</commit_message>
<xml_diff>
--- a/BBSalary_2022-08-22.xlsx
+++ b/BBSalary_2022-08-22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,69 +436,77 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Janet Apostol</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Rizalyn Repalda</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Janet Apostol</t>
-        </is>
+          <t>Gross Salary</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>7995</v>
+      </c>
+      <c r="C2" t="n">
+        <v>7995</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Gross Salary</t>
+          <t>PhilHealth Deduction</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7995</v>
+        <v>138.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>138.5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>PhilHealth Deduction</t>
+          <t>SSS Deduction</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>138.5</v>
+        <v>300</v>
+      </c>
+      <c r="C4" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>SSS Deduction</t>
+          <t>Pag-Ibig Deduction</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>300</v>
+        <v>50</v>
+      </c>
+      <c r="C5" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Pag-Ibig Deduction</t>
+          <t>Net Salary</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Net Salary</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+        <v>7506.5</v>
+      </c>
+      <c r="C6" t="n">
         <v>7506.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Made values round numbers (although this might make it more inaccurate, will find a fix) - Cleared up UI copy
</commit_message>
<xml_diff>
--- a/BBSalary_2022-08-22.xlsx
+++ b/BBSalary_2022-08-22.xlsx
@@ -452,10 +452,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7995</v>
+        <v>4264</v>
       </c>
       <c r="C2" t="n">
-        <v>7995</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="3">
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>138.5</v>
+        <v>73.87</v>
       </c>
       <c r="C3" t="n">
-        <v>138.5</v>
+        <v>36.93</v>
       </c>
     </row>
     <row r="4">
@@ -478,10 +478,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>300</v>
+        <v>160</v>
       </c>
       <c r="C4" t="n">
-        <v>300</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5">
@@ -491,10 +491,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>50</v>
+        <v>26.67</v>
       </c>
       <c r="C5" t="n">
-        <v>50</v>
+        <v>13.33</v>
       </c>
     </row>
     <row r="6">
@@ -504,10 +504,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7506.5</v>
+        <v>4003.47</v>
       </c>
       <c r="C6" t="n">
-        <v>7506.5</v>
+        <v>2001.73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>